<commit_message>
fixed topMost for EICs and sets
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB8E3D-00C4-4796-AB07-873639C36642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DB5A7A-CA77-4AFF-B6DA-60B7556CD28D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="6" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="130">
   <si>
     <t>[</t>
   </si>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577E9359-1D15-4F03-932A-97D98DDBC554}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,8 +971,11 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>52</v>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,6 +1037,9 @@
       <c r="D15" t="s">
         <v>48</v>
       </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1042,6 +1048,9 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1050,12 +1059,18 @@
       <c r="D17" t="s">
         <v>48</v>
       </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2616,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47284A1-E3D3-4291-B762-59F21D20AF3D}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
componentsNTSet class with plotGraph method
</commit_message>
<xml_diff>
--- a/set-impl.xlsx
+++ b/set-impl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Helmus\Documents\Rproj\patRoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0A357F-9CDC-4A4F-8E33-50A90B42140A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA999D4-E29E-41E4-BB7A-D3E9B8C1CC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4BFC050C-E8D8-4737-B5F4-2349612CBF83}"/>
   </bookViews>
   <sheets>
     <sheet name="fGroups" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="131">
   <si>
     <t>[</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>no, not really need for combined features atm other than input for fGroups</t>
+  </si>
+  <si>
+    <t>plotGraph</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577E9359-1D15-4F03-932A-97D98DDBC554}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -2230,15 +2233,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3C2673-B09C-47B8-945F-B7E3A2F3EE99}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2465,6 +2469,14 @@
         <v>48</v>
       </c>
       <c r="G19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>